<commit_message>
Add Digikey Cart Link
</commit_message>
<xml_diff>
--- a/Documentation/SST_BOM_v0.1.xlsx
+++ b/Documentation/SST_BOM_v0.1.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-RD/Shared Documents/Simple Switch Tester/Publishing/GitHub/Simple-Switch-Tester/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="11_C928632172BBFF291997287210CDEB7521C5B83F" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D0610D97-0463-40AB-95A1-891827695687}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="11_C928632172BBFF291997287210CDEB7521C5B83F" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{350B9033-68E6-4EB9-9106-0A80D262333A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1560" yWindow="1560" windowWidth="14970" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Individual Maker Purchase" sheetId="1" r:id="rId1"/>
     <sheet name="Bulk Purchase" sheetId="2" r:id="rId2"/>
     <sheet name="Comparison" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="93">
   <si>
     <t>Component</t>
   </si>
@@ -307,6 +307,12 @@
   <si>
     <t>$/ Pkg</t>
   </si>
+  <si>
+    <t>https://www.digikey.ca/short/47cdmb</t>
+  </si>
+  <si>
+    <t>Digikey Cart:</t>
+  </si>
 </sst>
 </file>
 
@@ -474,7 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -580,13 +586,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -599,6 +599,13 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -919,11 +926,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD999"/>
+  <dimension ref="A1:AE999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
+      <selection pane="bottomLeft" activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -942,73 +949,74 @@
     <col min="14" max="15" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" customWidth="1"/>
     <col min="17" max="17" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.7109375" customWidth="1"/>
-    <col min="19" max="19" width="25.7109375" customWidth="1"/>
-    <col min="20" max="20" width="7.42578125" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" style="43" customWidth="1"/>
+    <col min="19" max="19" width="31.7109375" customWidth="1"/>
+    <col min="20" max="20" width="25.7109375" customWidth="1"/>
+    <col min="21" max="21" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="K1" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="48" t="s">
+      <c r="M1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="46" t="s">
+      <c r="N1" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="46" t="s">
+      <c r="O1" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="46" t="s">
+      <c r="P1" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="46" t="s">
+      <c r="Q1" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="46" t="s">
+      <c r="R1" s="44"/>
+      <c r="S1" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="46" t="s">
+      <c r="T1" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="4"/>
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
@@ -1018,8 +1026,9 @@
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
-    </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE1" s="4"/>
+    </row>
+    <row r="2" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1027,7 +1036,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="51">
+      <c r="H2" s="49">
         <v>0.13</v>
       </c>
       <c r="I2" s="3"/>
@@ -1044,8 +1053,8 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="4"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="2"/>
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
@@ -1055,8 +1064,9 @@
       <c r="AB2" s="4"/>
       <c r="AC2" s="4"/>
       <c r="AD2" s="4"/>
-    </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE2" s="4"/>
+    </row>
+    <row r="3" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
@@ -1100,22 +1110,23 @@
       <c r="M3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
       <c r="P3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="Q3" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="R3" s="41"/>
+      <c r="S3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="S3" s="14" t="s">
+      <c r="T3" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>26</v>
       </c>
@@ -1156,22 +1167,23 @@
       <c r="M4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
       <c r="P4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="Q4" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="R4" s="13" t="s">
+      <c r="R4" s="41"/>
+      <c r="S4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="S4" s="14" t="s">
+      <c r="T4" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="7" t="s">
         <v>31</v>
@@ -1221,14 +1233,15 @@
       <c r="Q5" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="16" t="s">
+      <c r="R5" s="41"/>
+      <c r="S5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="S5" s="14" t="s">
+      <c r="T5" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="7" t="s">
         <v>36</v>
@@ -1278,14 +1291,15 @@
       <c r="Q6" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="R6" s="16" t="s">
+      <c r="R6" s="41"/>
+      <c r="S6" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="S6" s="14" t="s">
+      <c r="T6" s="14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="7" t="s">
         <v>79</v>
@@ -1335,14 +1349,15 @@
       <c r="Q7" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="R7" s="16" t="s">
+      <c r="R7" s="41"/>
+      <c r="S7" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="S7" s="18" t="s">
+      <c r="T7" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="7" t="s">
         <v>46</v>
@@ -1389,17 +1404,18 @@
       <c r="P8" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="Q8" s="50" t="s">
+      <c r="Q8" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="R8" s="16" t="s">
+      <c r="R8" s="48"/>
+      <c r="S8" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="S8" s="14" t="s">
+      <c r="T8" s="14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:30" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="29"/>
       <c r="B9" s="7"/>
       <c r="C9" s="26"/>
@@ -1417,11 +1433,16 @@
       <c r="O9" s="29"/>
       <c r="P9" s="19"/>
       <c r="Q9" s="19"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="14"/>
-    </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="43" t="s">
+      <c r="R9" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="S9" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="T9" s="14"/>
+    </row>
+    <row r="10" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="50" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1462,11 +1483,12 @@
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
-      <c r="R10" s="16"/>
+      <c r="R10" s="29"/>
       <c r="S10" s="16"/>
-    </row>
-    <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="44"/>
+      <c r="T10" s="16"/>
+    </row>
+    <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="51"/>
       <c r="B11" s="7" t="s">
         <v>54</v>
       </c>
@@ -1505,11 +1527,12 @@
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
-      <c r="R11" s="16"/>
+      <c r="R11" s="29"/>
       <c r="S11" s="16"/>
-    </row>
-    <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="44"/>
+      <c r="T11" s="16"/>
+    </row>
+    <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="51"/>
       <c r="B12" s="7" t="s">
         <v>55</v>
       </c>
@@ -1548,10 +1571,11 @@
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
-      <c r="R12" s="16"/>
+      <c r="R12" s="29"/>
       <c r="S12" s="16"/>
-    </row>
-    <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T12" s="16"/>
+    </row>
+    <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>56</v>
       </c>
@@ -1593,18 +1617,20 @@
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="12"/>
-      <c r="R13" s="16"/>
+      <c r="R13" s="29"/>
       <c r="S13" s="16"/>
-    </row>
-    <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T13" s="16"/>
+    </row>
+    <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
-      <c r="R14" s="16"/>
+      <c r="R14" s="29"/>
       <c r="S14" s="16"/>
-    </row>
-    <row r="15" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T14" s="16"/>
+    </row>
+    <row r="15" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
         <v>58</v>
       </c>
@@ -1625,10 +1651,11 @@
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
-      <c r="R15" s="16"/>
+      <c r="R15" s="29"/>
       <c r="S15" s="16"/>
-    </row>
-    <row r="16" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T15" s="16"/>
+    </row>
+    <row r="16" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
         <v>60</v>
       </c>
@@ -1649,10 +1676,11 @@
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="12"/>
-      <c r="R16" s="16"/>
+      <c r="R16" s="29"/>
       <c r="S16" s="16"/>
-    </row>
-    <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T16" s="16"/>
+    </row>
+    <row r="17" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="C17" s="25"/>
@@ -1669,10 +1697,11 @@
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
       <c r="Q17" s="12"/>
-      <c r="R17" s="16"/>
+      <c r="R17" s="29"/>
       <c r="S17" s="16"/>
-    </row>
-    <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T17" s="16"/>
+    </row>
+    <row r="18" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="25"/>
@@ -1689,10 +1718,11 @@
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
       <c r="Q18" s="12"/>
-      <c r="R18" s="16"/>
+      <c r="R18" s="29"/>
       <c r="S18" s="16"/>
-    </row>
-    <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T18" s="16"/>
+    </row>
+    <row r="19" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="25"/>
@@ -1709,10 +1739,11 @@
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
       <c r="Q19" s="12"/>
-      <c r="R19" s="16"/>
+      <c r="R19" s="29"/>
       <c r="S19" s="16"/>
-    </row>
-    <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T19" s="16"/>
+    </row>
+    <row r="20" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="12"/>
       <c r="C20" s="25"/>
       <c r="E20" s="8"/>
@@ -1724,17 +1755,17 @@
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
-      <c r="R20" s="16"/>
       <c r="S20" s="16"/>
-    </row>
-    <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T20" s="16"/>
+    </row>
+    <row r="21" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="25"/>
-      <c r="R21" s="16"/>
       <c r="S21" s="16"/>
-    </row>
-    <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T21" s="16"/>
+    </row>
+    <row r="22" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="25"/>
@@ -1751,10 +1782,11 @@
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
       <c r="Q22" s="12"/>
-      <c r="R22" s="16"/>
+      <c r="R22" s="29"/>
       <c r="S22" s="16"/>
-    </row>
-    <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T22" s="16"/>
+    </row>
+    <row r="23" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="25"/>
@@ -1771,10 +1803,11 @@
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
       <c r="Q23" s="12"/>
-      <c r="R23" s="16"/>
+      <c r="R23" s="29"/>
       <c r="S23" s="16"/>
-    </row>
-    <row r="24" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T23" s="16"/>
+    </row>
+    <row r="24" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="25"/>
@@ -1791,10 +1824,11 @@
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="12"/>
-      <c r="R24" s="16"/>
+      <c r="R24" s="29"/>
       <c r="S24" s="16"/>
-    </row>
-    <row r="25" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T24" s="16"/>
+    </row>
+    <row r="25" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="25"/>
@@ -1807,10 +1841,10 @@
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="O25" s="12"/>
-      <c r="R25" s="16"/>
       <c r="S25" s="16"/>
-    </row>
-    <row r="26" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T25" s="16"/>
+    </row>
+    <row r="26" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="25"/>
@@ -1824,10 +1858,10 @@
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="O26" s="12"/>
-      <c r="R26" s="16"/>
       <c r="S26" s="16"/>
-    </row>
-    <row r="27" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T26" s="16"/>
+    </row>
+    <row r="27" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="25"/>
@@ -1841,10 +1875,10 @@
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
       <c r="O27" s="12"/>
-      <c r="R27" s="16"/>
       <c r="S27" s="16"/>
-    </row>
-    <row r="28" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T27" s="16"/>
+    </row>
+    <row r="28" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="25"/>
@@ -1858,10 +1892,10 @@
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
       <c r="O28" s="12"/>
-      <c r="R28" s="16"/>
       <c r="S28" s="16"/>
-    </row>
-    <row r="29" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T28" s="16"/>
+    </row>
+    <row r="29" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="25"/>
@@ -1875,10 +1909,10 @@
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
       <c r="O29" s="12"/>
-      <c r="R29" s="16"/>
       <c r="S29" s="16"/>
-    </row>
-    <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T29" s="16"/>
+    </row>
+    <row r="30" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="25"/>
@@ -1892,10 +1926,10 @@
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
       <c r="O30" s="12"/>
-      <c r="R30" s="16"/>
       <c r="S30" s="16"/>
-    </row>
-    <row r="31" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T30" s="16"/>
+    </row>
+    <row r="31" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
       <c r="C31" s="25"/>
@@ -1909,10 +1943,10 @@
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
       <c r="O31" s="12"/>
-      <c r="R31" s="16"/>
       <c r="S31" s="16"/>
-    </row>
-    <row r="32" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T31" s="16"/>
+    </row>
+    <row r="32" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="C32" s="25"/>
@@ -1926,10 +1960,10 @@
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
       <c r="O32" s="12"/>
-      <c r="R32" s="16"/>
       <c r="S32" s="16"/>
-    </row>
-    <row r="33" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T32" s="16"/>
+    </row>
+    <row r="33" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
       <c r="C33" s="25"/>
@@ -1943,10 +1977,10 @@
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
       <c r="O33" s="12"/>
-      <c r="R33" s="16"/>
       <c r="S33" s="16"/>
-    </row>
-    <row r="34" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T33" s="16"/>
+    </row>
+    <row r="34" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="C34" s="25"/>
@@ -1960,10 +1994,10 @@
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="O34" s="12"/>
-      <c r="R34" s="16"/>
       <c r="S34" s="16"/>
-    </row>
-    <row r="35" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T34" s="16"/>
+    </row>
+    <row r="35" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="C35" s="25"/>
@@ -1977,10 +2011,10 @@
       <c r="L35" s="10"/>
       <c r="M35" s="10"/>
       <c r="O35" s="12"/>
-      <c r="R35" s="16"/>
       <c r="S35" s="16"/>
-    </row>
-    <row r="36" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T35" s="16"/>
+    </row>
+    <row r="36" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="C36" s="25"/>
@@ -1994,10 +2028,10 @@
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
       <c r="O36" s="12"/>
-      <c r="R36" s="16"/>
       <c r="S36" s="16"/>
-    </row>
-    <row r="37" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T36" s="16"/>
+    </row>
+    <row r="37" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="25"/>
@@ -2011,10 +2045,10 @@
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
       <c r="O37" s="12"/>
-      <c r="R37" s="16"/>
       <c r="S37" s="16"/>
-    </row>
-    <row r="38" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T37" s="16"/>
+    </row>
+    <row r="38" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="12"/>
       <c r="B38" s="12"/>
       <c r="C38" s="25"/>
@@ -2028,10 +2062,10 @@
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
       <c r="O38" s="12"/>
-      <c r="R38" s="16"/>
       <c r="S38" s="16"/>
-    </row>
-    <row r="39" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="T38" s="16"/>
+    </row>
+    <row r="39" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="25"/>
@@ -2045,10 +2079,10 @@
       <c r="L39" s="10"/>
       <c r="M39" s="10"/>
       <c r="O39" s="12"/>
-      <c r="R39" s="16"/>
       <c r="S39" s="16"/>
-    </row>
-    <row r="40" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="T39" s="16"/>
+    </row>
+    <row r="40" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="12"/>
       <c r="B40" s="12"/>
       <c r="C40" s="25"/>
@@ -2062,10 +2096,10 @@
       <c r="L40" s="10"/>
       <c r="M40" s="10"/>
       <c r="O40" s="12"/>
-      <c r="R40" s="16"/>
       <c r="S40" s="16"/>
-    </row>
-    <row r="41" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="T40" s="16"/>
+    </row>
+    <row r="41" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="12"/>
       <c r="B41" s="12"/>
       <c r="C41" s="25"/>
@@ -2079,10 +2113,10 @@
       <c r="L41" s="10"/>
       <c r="M41" s="10"/>
       <c r="O41" s="12"/>
-      <c r="R41" s="16"/>
       <c r="S41" s="16"/>
-    </row>
-    <row r="42" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="T41" s="16"/>
+    </row>
+    <row r="42" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="25"/>
@@ -2096,10 +2130,10 @@
       <c r="L42" s="10"/>
       <c r="M42" s="10"/>
       <c r="O42" s="12"/>
-      <c r="R42" s="16"/>
       <c r="S42" s="16"/>
-    </row>
-    <row r="43" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="T42" s="16"/>
+    </row>
+    <row r="43" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="25"/>
@@ -2113,10 +2147,10 @@
       <c r="L43" s="10"/>
       <c r="M43" s="10"/>
       <c r="O43" s="12"/>
-      <c r="R43" s="16"/>
       <c r="S43" s="16"/>
-    </row>
-    <row r="44" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="T43" s="16"/>
+    </row>
+    <row r="44" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C44" s="27"/>
       <c r="E44" s="26"/>
       <c r="F44" s="10"/>
@@ -2129,7 +2163,7 @@
       <c r="M44" s="10"/>
       <c r="O44" s="12"/>
     </row>
-    <row r="45" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E45" s="26"/>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
@@ -2141,7 +2175,7 @@
       <c r="M45" s="10"/>
       <c r="O45" s="12"/>
     </row>
-    <row r="46" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="C46" s="25"/>
@@ -2155,10 +2189,10 @@
       <c r="L46" s="10"/>
       <c r="M46" s="10"/>
       <c r="O46" s="12"/>
-      <c r="R46" s="16"/>
       <c r="S46" s="16"/>
-    </row>
-    <row r="47" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="T46" s="16"/>
+    </row>
+    <row r="47" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="C47" s="25"/>
@@ -2172,10 +2206,10 @@
       <c r="L47" s="10"/>
       <c r="M47" s="10"/>
       <c r="O47" s="12"/>
-      <c r="R47" s="16"/>
       <c r="S47" s="16"/>
-    </row>
-    <row r="48" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="T47" s="16"/>
+    </row>
+    <row r="48" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="C48" s="25"/>
@@ -2189,8 +2223,8 @@
       <c r="L48" s="10"/>
       <c r="M48" s="10"/>
       <c r="O48" s="12"/>
-      <c r="R48" s="16"/>
       <c r="S48" s="16"/>
+      <c r="T48" s="16"/>
     </row>
     <row r="49" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C49" s="27"/>
@@ -14320,16 +14354,16 @@
     <mergeCell ref="A10:A12"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="R3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="S3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="R4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="S4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="R5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="S5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="R6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="S6" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="R7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="S7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="S3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="T3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="S4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="T4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="S5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="T5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="S6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="T6" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="S7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="T7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -25903,10 +25937,10 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="44"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="3"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -31847,9 +31881,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -32070,19 +32107,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{025671EA-916B-4F13-B35F-A54AB9C41265}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C99630-F150-4BD3-B1AF-50D044F731DA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -32107,9 +32140,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C99630-F150-4BD3-B1AF-50D044F731DA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{025671EA-916B-4F13-B35F-A54AB9C41265}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>